<commit_message>
new changes in homepage
</commit_message>
<xml_diff>
--- a/MYFramework/src/main/java/helper/exceldata/Frameworkworksheet.xlsx
+++ b/MYFramework/src/main/java/helper/exceldata/Frameworkworksheet.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>Username</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>https://performancemanager8.successfactors.com/sf/home?bplte_company=BPOCUSTOM10#Shell-home</t>
+  </si>
+  <si>
+    <t>Message</t>
   </si>
 </sst>
 </file>
@@ -553,11 +556,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -565,7 +566,7 @@
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -575,8 +576,11 @@
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -587,7 +591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
NewPages-LearningPage and RequestforTest classes created, added new tab in testdata xlsx file.
</commit_message>
<xml_diff>
--- a/MYFramework/src/main/java/helper/exceldata/Frameworkworksheet.xlsx
+++ b/MYFramework/src/main/java/helper/exceldata/Frameworkworksheet.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parag.borawake\git\NewFrameworks_1\MYFramework\src\main\java\helper\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3020713-1024-4AA3-A286-4F4C5CF17787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4BE01F-AAEF-4C30-83AA-E9DC788F03EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="LMS" sheetId="6" r:id="rId2"/>
     <sheet name="HomePage" sheetId="2" r:id="rId3"/>
-    <sheet name="CreateRequisition" sheetId="3" r:id="rId4"/>
-    <sheet name="AddNewEmployee" sheetId="4" r:id="rId5"/>
-    <sheet name="AddNewEmployeeTest" sheetId="5" r:id="rId6"/>
+    <sheet name="LearningPage" sheetId="7" r:id="rId4"/>
+    <sheet name="CreateRequisition" sheetId="3" r:id="rId5"/>
+    <sheet name="AddNewEmployee" sheetId="4" r:id="rId6"/>
+    <sheet name="AddNewEmployeeTest" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>Username</t>
   </si>
@@ -189,6 +190,12 @@
   </si>
   <si>
     <t>ClassesText</t>
+  </si>
+  <si>
+    <t>SearchBox</t>
+  </si>
+  <si>
+    <t>PassportTraining</t>
   </si>
 </sst>
 </file>
@@ -631,7 +638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3606D91B-2CAB-45D0-84DF-071D6DC42850}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
@@ -688,6 +695,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E086AC3-3D27-4938-A6D5-EFCCF5BDF4E8}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
@@ -868,7 +904,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -911,7 +947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>

</xml_diff>